<commit_message>
Fix styling and logic for action screens, and correct integer options
</commit_message>
<xml_diff>
--- a/app/config/tables/business/forms/authorization/authorization.xlsx
+++ b/app/config/tables/business/forms/authorization/authorization.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clarice\eKichabi\app-designer\app\config\tables\business\forms\authorization\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="37935" windowHeight="19695" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,7 @@
     <sheet name="settings" sheetId="5" r:id="rId4"/>
     <sheet name="model" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="80">
   <si>
     <t>comments</t>
   </si>
@@ -145,12 +140,6 @@
   </si>
   <si>
     <t>select_one_integer</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>male_female</t>
@@ -284,7 +273,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -373,7 +362,6 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -383,6 +371,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -797,24 +786,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" customWidth="1"/>
-    <col min="7" max="8" width="41.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" customWidth="1"/>
+    <col min="6" max="6" width="31.5" customWidth="1"/>
+    <col min="7" max="8" width="41.5" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="1023" width="11.28515625" customWidth="1"/>
+    <col min="11" max="1023" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -855,7 +844,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="D2" t="s">
         <v>24</v>
       </c>
@@ -863,10 +852,10 @@
         <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="D3" t="s">
         <v>22</v>
       </c>
@@ -874,27 +863,27 @@
         <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="36">
       <c r="D4" t="s">
         <v>13</v>
       </c>
       <c r="E4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" t="s">
-        <v>72</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:13">
       <c r="D5" s="7" t="s">
         <v>37</v>
       </c>
@@ -902,7 +891,7 @@
         <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G5" t="s">
         <v>33</v>
@@ -927,44 +916,49 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="1" max="1" width="36.5" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="55.7109375" customWidth="1"/>
+    <col min="4" max="4" width="55.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="10" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="83.25" customHeight="1">
+      <c r="A2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>78</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -972,19 +966,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD30"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="44.140625" customWidth="1"/>
-    <col min="4" max="1024" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" customWidth="1"/>
+    <col min="3" max="3" width="44.1640625" customWidth="1"/>
+    <col min="4" max="1024" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="16.25" customHeight="1">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -995,9 +989,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="18" customHeight="1">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
@@ -1006,9 +1000,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="16" customHeight="1">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
@@ -1017,9 +1011,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17" customHeight="1">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
         <v>27</v>
@@ -1028,54 +1022,54 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="16" customHeight="1">
       <c r="A6" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>38</v>
+      <c r="B6" s="11">
+        <v>0</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="17" customHeight="1">
       <c r="A7" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>39</v>
+      <c r="B7" s="11">
+        <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="19" customHeight="1"/>
+    <row r="9" spans="1:3" ht="15" customHeight="1">
       <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
         <v>40</v>
       </c>
-      <c r="B9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>42</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1092,15 +1086,15 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
-    <col min="4" max="1022" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="4" max="1022" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="16.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -1111,15 +1105,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="16.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -1127,7 +1121,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="16.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -1135,12 +1129,12 @@
         <v>20180703</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="16.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1162,149 +1156,149 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>53</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
         <v>59</v>
       </c>
-      <c r="B9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1312,7 +1306,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1320,31 +1314,36 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor logic to reduce duplicate code, include unsure option as verification/authorization choice
</commit_message>
<xml_diff>
--- a/app/config/tables/business/forms/authorization/authorization.xlsx
+++ b/app/config/tables/business/forms/authorization/authorization.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="5320" yWindow="760" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="81">
   <si>
     <t>comments</t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>Has the VEO authorized this business?</t>
-  </si>
-  <si>
-    <t>true_false</t>
   </si>
   <si>
     <t>True</t>
@@ -268,6 +265,12 @@
   </si>
   <si>
     <t>choice_item.village === data('village')</t>
+  </si>
+  <si>
+    <t>true_false_unsure</t>
+  </si>
+  <si>
+    <t>Unsure</t>
   </si>
 </sst>
 </file>
@@ -852,7 +855,7 @@
         <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -863,7 +866,7 @@
         <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="36">
@@ -871,27 +874,27 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="D5" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5" t="s">
         <v>33</v>
@@ -926,30 +929,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="83.25" customHeight="1">
       <c r="A2" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>77</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -964,10 +967,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -991,7 +994,7 @@
     </row>
     <row r="2" spans="1:3" ht="18" customHeight="1">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
@@ -1002,7 +1005,7 @@
     </row>
     <row r="3" spans="1:3" ht="16" customHeight="1">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
@@ -1013,7 +1016,7 @@
     </row>
     <row r="4" spans="1:3" ht="17" customHeight="1">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
         <v>27</v>
@@ -1024,47 +1027,58 @@
     </row>
     <row r="6" spans="1:3" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="B6" s="11">
         <v>0</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" customHeight="1">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="B7" s="11">
         <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="19" customHeight="1"/>
-    <row r="9" spans="1:3" ht="15" customHeight="1">
-      <c r="A9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="19" customHeight="1">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8">
+        <v>-1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="19" customHeight="1"/>
+    <row r="10" spans="1:3" ht="15" customHeight="1">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1110,7 +1124,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16.75" customHeight="1">
@@ -1134,7 +1148,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1175,7 +1189,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1183,7 +1197,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1191,23 +1205,23 @@
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
         <v>51</v>
-      </c>
-      <c r="B5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
         <v>53</v>
-      </c>
-      <c r="B6" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1215,7 +1229,7 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1223,23 +1237,23 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
         <v>57</v>
-      </c>
-      <c r="B9" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1247,7 +1261,7 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1255,7 +1269,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1263,7 +1277,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1271,7 +1285,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1279,7 +1293,7 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1287,15 +1301,15 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1319,15 +1333,15 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1335,7 +1349,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>